<commit_message>
taxon author tolerance and more
</commit_message>
<xml_diff>
--- a/app_kit/tests/TESTS_ROOT/xlsx_for_testing/TaxonProfiles/invalid/Taxon profiles.xlsx
+++ b/app_kit/tests/TESTS_ROOT/xlsx_for_testing/TaxonProfiles/invalid/Taxon profiles.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Taxon Profiles" sheetId="1" state="visible" r:id="rId3"/>
@@ -29,7 +29,7 @@
     <t xml:space="preserve">Author (optional)</t>
   </si>
   <si>
-    <t xml:space="preserve">Morphotype</t>
+    <t xml:space="preserve">Morphotype (optional)</t>
   </si>
   <si>
     <t xml:space="preserve">short_profile</t>
@@ -532,8 +532,8 @@
   </sheetPr>
   <dimension ref="A1:AMR27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3979,9 +3979,8 @@
       <c r="L27" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="F5:H5"/>
-    <mergeCell ref="I5:L5"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -4000,7 +3999,7 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>